<commit_message>
Atualiza notas dos alunos
</commit_message>
<xml_diff>
--- a/_pedro/notas/musa86.xlsx
+++ b/_pedro/notas/musa86.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kroger/Code/genosmus/_pedro/notas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03330C4-9461-A94E-9833-C4D2B0666FE2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBFE269-9228-904E-8C5C-F62D8BCDD63A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{0F653A56-3787-D649-A495-8EB2FAFB69E3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{0F653A56-3787-D649-A495-8EB2FAFB69E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,9 +484,12 @@
       <c r="B2">
         <v>1.25</v>
       </c>
+      <c r="C2">
+        <v>1.25</v>
+      </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -496,9 +499,12 @@
       <c r="B3">
         <v>1.25</v>
       </c>
+      <c r="C3">
+        <v>1.25</v>
+      </c>
       <c r="I3">
         <f t="shared" ref="I3:I7" si="0">SUM(B3:H3)</f>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -508,9 +514,12 @@
       <c r="B4">
         <v>1.25</v>
       </c>
+      <c r="C4">
+        <v>1.25</v>
+      </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -520,6 +529,9 @@
       <c r="B5">
         <v>0</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -532,6 +544,9 @@
       <c r="B6">
         <v>0</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -544,9 +559,12 @@
       <c r="B7">
         <v>1.25</v>
       </c>
+      <c r="C7">
+        <v>1.25</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>